<commit_message>
read from spreadsheet complete
</commit_message>
<xml_diff>
--- a/WiltyData.xlsx
+++ b/WiltyData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11660" windowHeight="16260" tabRatio="500"/>
+    <workbookView xWindow="14060" yWindow="0" windowWidth="11660" windowHeight="16260" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="9">
   <si>
     <t>Season</t>
   </si>
@@ -30,12 +30,6 @@
     <t>Who</t>
   </si>
   <si>
-    <t>David</t>
-  </si>
-  <si>
-    <t>Lee</t>
-  </si>
-  <si>
     <t>Answer</t>
   </si>
   <si>
@@ -51,7 +45,7 @@
     <t>F</t>
   </si>
   <si>
-    <t>Test</t>
+    <t>Correct</t>
   </si>
 </sst>
 </file>
@@ -420,15 +414,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -442,53 +436,44 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3">
-        <v>0</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
+      <c r="D3" t="s">
+        <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4">
         <v>1</v>
       </c>
@@ -496,33 +481,33 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
         <v>6</v>
       </c>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5" t="s">
-        <v>8</v>
+      <c r="D5" t="s">
+        <v>5</v>
       </c>
       <c r="E5" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6">
         <v>1</v>
       </c>
@@ -530,13 +515,115 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
         <v>6</v>
       </c>
-      <c r="D6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" t="s">
-        <v>9</v>
+      <c r="D7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
filling in data array
</commit_message>
<xml_diff>
--- a/WiltyData.xlsx
+++ b/WiltyData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="14060" yWindow="0" windowWidth="11660" windowHeight="16260" tabRatio="500"/>
+    <workbookView xWindow="16400" yWindow="0" windowWidth="12140" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -414,10 +414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -624,6 +624,54 @@
       </c>
       <c r="E12" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>